<commit_message>
Save differences from MO 04/09
</commit_message>
<xml_diff>
--- a/templates/simple_payment_list.xlsx
+++ b/templates/simple_payment_list.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>date</t>
   </si>
@@ -198,6 +198,9 @@
     <t>You can enter simple transaction here.  
 Some data restrictions are enforced
 Please remember to save before exiting.</t>
+  </si>
+  <si>
+    <t>use_cell</t>
   </si>
 </sst>
 </file>
@@ -235,7 +238,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -335,7 +338,29 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color auto="1"/>
       </right>
       <top style="medium">
@@ -350,37 +375,47 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color auto="1"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color auto="1"/>
       </right>
       <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -395,12 +430,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -678,25 +717,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:H103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="56" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
       <c r="F1" s="13"/>
-    </row>
-    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="14"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -715,16 +759,19 @@
       <c r="F2" s="10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="15"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -732,7 +779,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -740,7 +787,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -748,7 +795,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -756,7 +803,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -764,7 +811,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -772,7 +819,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -780,7 +827,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -788,7 +835,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -796,7 +843,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -804,7 +851,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -812,7 +859,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -820,7 +867,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -844,28 +891,693 @@
       <c r="E18" s="2"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="7"/>
+    <row r="19" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="15"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="17"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="3"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="3"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="3"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="3"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="3"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="3"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="3"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="3"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="3"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="3"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="3"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="3"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="3"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="3"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="3"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="3"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="3"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="3"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="4"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="3"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="4"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="3"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="3"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="3"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="3"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="4"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="3"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="4"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="3"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="4"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="3"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="4"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="3"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="4"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="3"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="4"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="3"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="4"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="3"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="4"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="3"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="4"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="3"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="4"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="3"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="4"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="3"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="4"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="3"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="4"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="3"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="4"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="3"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="4"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="3"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="4"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="3"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="4"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="3"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
+      <c r="F69" s="4"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="3"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="4"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="3"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
+      <c r="F71" s="4"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="3"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="4"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="3"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="4"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="3"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="4"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="3"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="4"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="3"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="4"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="3"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="4"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="3"/>
+      <c r="B78" s="2"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="4"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="3"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="4"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="3"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="4"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="3"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="4"/>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="3"/>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="4"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="3"/>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="4"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="3"/>
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="4"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="3"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="4"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="3"/>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="2"/>
+      <c r="F86" s="4"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="3"/>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="2"/>
+      <c r="F87" s="4"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="3"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="4"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="3"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="4"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="3"/>
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="4"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="3"/>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
+      <c r="D91" s="2"/>
+      <c r="E91" s="2"/>
+      <c r="F91" s="4"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="3"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+      <c r="D92" s="2"/>
+      <c r="E92" s="2"/>
+      <c r="F92" s="4"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="3"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+      <c r="E93" s="2"/>
+      <c r="F93" s="4"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="3"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="4"/>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="3"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="4"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="3"/>
+      <c r="B96" s="2"/>
+      <c r="C96" s="2"/>
+      <c r="D96" s="2"/>
+      <c r="E96" s="2"/>
+      <c r="F96" s="4"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="3"/>
+      <c r="B97" s="2"/>
+      <c r="C97" s="2"/>
+      <c r="D97" s="2"/>
+      <c r="E97" s="2"/>
+      <c r="F97" s="4"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="3"/>
+      <c r="B98" s="2"/>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="4"/>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" s="3"/>
+      <c r="B99" s="2"/>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
+      <c r="E99" s="2"/>
+      <c r="F99" s="4"/>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" s="3"/>
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
+      <c r="E100" s="2"/>
+      <c r="F100" s="4"/>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="3"/>
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="4"/>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" s="3"/>
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="4"/>
+    </row>
+    <row r="103" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="5"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="7"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
@@ -873,19 +1585,19 @@
           <x14:formula1>
             <xm:f>Sheet2!$D$2:$D$16</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D22</xm:sqref>
+          <xm:sqref>D3:D103</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Select Transaction Type" error="You must select one of the pre-defined transaction types.">
           <x14:formula1>
             <xm:f>Sheet2!$E$2:$E$25</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E22</xm:sqref>
+          <xm:sqref>E3:E103</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Select Money Pot" error="Select one of the predefined money pots where the money came form.">
           <x14:formula1>
             <xm:f>Sheet2!$F$2:$F$14</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F22</xm:sqref>
+          <xm:sqref>F3:F103</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Enter sensible Date" error="The given date should be after 2013 and not more than 6 months into the future.">
           <x14:formula1>
@@ -894,7 +1606,7 @@
           <x14:formula2>
             <xm:f>Sheet2!A3</xm:f>
           </x14:formula2>
-          <xm:sqref>A3:A22</xm:sqref>
+          <xm:sqref>A3:A103</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Enter Sensible Amount" error="Only transaction values below 10.000 are allowed.">
           <x14:formula1>
@@ -958,7 +1670,7 @@
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <f ca="1">TODAY()+180</f>
-        <v>43145</v>
+        <v>43162</v>
       </c>
       <c r="C3">
         <v>10000</v>

</xml_diff>